<commit_message>
updates scaling logic (added x-axis scaling factor)
</commit_message>
<xml_diff>
--- a/modules/area_estimation/3280x2464/ScalingFactor.xlsx
+++ b/modules/area_estimation/3280x2464/ScalingFactor.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\GitHub\ai-pothole-models\modules\area_estimation\3280x2464\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01530CD8-63DF-4822-A99B-2CACC4DBF972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E570D10E-D177-4C60-8674-BF356855C292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="y-scaling factor" sheetId="1" r:id="rId1"/>
+    <sheet name="x-scaling factor" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>Rectangle</t>
   </si>
@@ -142,16 +143,90 @@
   <si>
     <t>Scaling Factor Needed
 (m^2/pixel^2)</t>
+  </si>
+  <si>
+    <t>pt1</t>
+  </si>
+  <si>
+    <t>(3187.6, 2464.0)</t>
+  </si>
+  <si>
+    <t>pt2</t>
+  </si>
+  <si>
+    <t>x2-x1</t>
+  </si>
+  <si>
+    <t>y2-y1</t>
+  </si>
+  <si>
+    <t>area in pixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y distance </t>
+  </si>
+  <si>
+    <t>scaling factor</t>
+  </si>
+  <si>
+    <t>FINAL AREA</t>
+  </si>
+  <si>
+    <t>210.3, 11.29</t>
+  </si>
+  <si>
+    <t>714.7, 606.91, 978.96, 652.99</t>
+  </si>
+  <si>
+    <t>THIRD ROW</t>
+  </si>
+  <si>
+    <t>CENTER COLUMN</t>
+  </si>
+  <si>
+    <t>x-axis distance from camera
+(pixels)</t>
+  </si>
+  <si>
+    <t>(138, 981)</t>
+  </si>
+  <si>
+    <t>(759, 981)</t>
+  </si>
+  <si>
+    <t>(1212, 1038)</t>
+  </si>
+  <si>
+    <t>(696, 1038)</t>
+  </si>
+  <si>
+    <t>(1467, 981)</t>
+  </si>
+  <si>
+    <t>(1821, 1038)</t>
+  </si>
+  <si>
+    <t>(2010, 981)</t>
+  </si>
+  <si>
+    <t>(2454, 1038)</t>
+  </si>
+  <si>
+    <t>(2586, 981)</t>
+  </si>
+  <si>
+    <t>(3162, 1038)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="179" formatCode="0.0000000000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,13 +242,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -188,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -219,6 +308,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -317,7 +409,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$16</c:f>
+              <c:f>'y-scaling factor'!$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -437,7 +529,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$23</c:f>
+              <c:f>'y-scaling factor'!$C$17:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -467,7 +559,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$23</c:f>
+              <c:f>'y-scaling factor'!$D$17:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000000000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -499,6 +591,67 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-82C2-4D36-A40A-793876FDF146}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>bla</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'y-scaling factor'!$M$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>742.61500000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'y-scaling factor'!$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.7747708563198579E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4D86-4565-8348-7F6E259DE558}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -561,12 +714,6 @@
                   <a:rPr lang="en-CA" baseline="0"/>
                   <a:t> from camera y-axis (pixels)</a:t>
                 </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:endParaRPr lang="en-CA"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -686,7 +833,16 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-CA" baseline="0"/>
-                  <a:t> (m2/pixel)</a:t>
+                  <a:t> (m2/pixel^2</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-CA"/>
               </a:p>
@@ -807,7 +963,722 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1320" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Scaling</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Factor Needed (m2/pixel^2)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1320" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'x-scaling factor'!$E$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scaling Factor Needed
+(m2/pixel)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'x-scaling factor'!$D$17:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>986</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1644</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2232</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2874</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'x-scaling factor'!$E$17:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.8601521725460613E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6820417489640218E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2389731390623451E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.0000000000000000">
+                  <c:v>9.8782993519835626E-6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0000000000000000">
+                  <c:v>7.6145224171539957E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A56F-432C-87CF-57B13FFBBF31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1811549279"/>
+        <c:axId val="1811549759"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>rise</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:trendline>
+                  <c:spPr>
+                    <a:ln w="19050" cap="rnd">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:trendlineType val="linear"/>
+                  <c:dispRSqr val="0"/>
+                  <c:dispEq val="1"/>
+                  <c:trendlineLbl>
+                    <c:numFmt formatCode="General" sourceLinked="0"/>
+                    <c:spPr>
+                      <a:noFill/>
+                      <a:ln>
+                        <a:noFill/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                    <c:txPr>
+                      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                      <a:lstStyle/>
+                      <a:p>
+                        <a:pPr>
+                          <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:defRPr>
+                        </a:pPr>
+                        <a:endParaRPr lang="en-US"/>
+                      </a:p>
+                    </c:txPr>
+                  </c:trendlineLbl>
+                </c:trendline>
+                <c:xVal>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'x-scaling factor'!$D$16:$D$19</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>x-axis distance from camera
+(pixels)</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>417</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>986</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1644</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'x-scaling factor'!$E$16:$E$19</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.000000000000000</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0" formatCode="General">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>7.8601521725460613E-6</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>9.6820417489640218E-6</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.2389731390623451E-5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000006-A56F-432C-87CF-57B13FFBBF31}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>fall</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'x-scaling factor'!$B$16:$B$19</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>x-axis distance from camera
+(pixels)</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1644</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2232</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2874</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'x-scaling factor'!$C$16:$C$19</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.000000000000000</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0" formatCode="General">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.2389731390623451E-5</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="0.0000000000000000">
+                        <c:v>9.8782993519835626E-6</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="0.0000000000000000">
+                        <c:v>7.6145224171539957E-6</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000A-A56F-432C-87CF-57B13FFBBF31}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1811549279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Distance from camera x-axis (pixels)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1811549759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1811549759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Scaling Factor (m2/pixel^2)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000000000000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1811549279"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100" b="1">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1363,6 +2234,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1384,6 +2771,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB961356-42CE-C214-08C8-6ED8C7A36B72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>625959</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142898</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1942296</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>112922</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62D74A63-FB7F-B845-FA12-2C9CF2C47A94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1667,14 +3095,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.06640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
@@ -1683,13 +3112,20 @@
     <col min="7" max="7" width="22.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1714,8 +3150,14 @@
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1743,8 +3185,14 @@
         <f>G3/F3</f>
         <v>1.1098247009688326E-7</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1772,8 +3220,17 @@
         <f t="shared" ref="H4:H9" si="1">G4/F4</f>
         <v>3.3379619739371929E-6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1802,8 +3259,20 @@
         <v>1.3354700854700855E-5</v>
       </c>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K5">
+        <f>572.06-78.04</f>
+        <v>494.01999999999992</v>
+      </c>
+      <c r="L5">
+        <f>781.95-703.28</f>
+        <v>78.670000000000073</v>
+      </c>
+      <c r="M5">
+        <f>(703.28+781.95)/2</f>
+        <v>742.61500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1833,7 +3302,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1862,8 +3331,17 @@
         <v>1.0121457489878542E-4</v>
       </c>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1892,8 +3370,20 @@
         <v>1.8037518037518038E-4</v>
       </c>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K8">
+        <f>K5*L5</f>
+        <v>38864.553400000033</v>
+      </c>
+      <c r="L8">
+        <f>G17/(G18+G19*(M5)+G20*(M5*M5))</f>
+        <v>7.7747708563198579E-5</v>
+      </c>
+      <c r="M8">
+        <f>K8*L8</f>
+        <v>3.0216299711820711</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1923,7 +3413,26 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="J14">
+        <f>978.96-714.7</f>
+        <v>264.26</v>
+      </c>
+      <c r="K14">
+        <f>652.99-606.91</f>
+        <v>46.080000000000041</v>
+      </c>
+      <c r="L14">
+        <f>J14*K14</f>
+        <v>12177.100800000011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C16" s="4" t="s">
         <v>25</v>
       </c>
@@ -1946,8 +3455,8 @@
         <v>-2.2788150560381401E-4</v>
       </c>
       <c r="H17">
-        <f>G17/(G18+G19*(C3)+G20*(C3*C3))</f>
-        <v>4.7384404867829322E-7</v>
+        <f>G17/(G18+G19*(M5)+G20*(M5*M5))</f>
+        <v>7.7747708563198579E-5</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.45">
@@ -2029,6 +3538,423 @@
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D27" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1E50E9-E4C9-46DC-A3D5-132ED23BE96B}">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.73046875" customWidth="1"/>
+    <col min="7" max="7" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>417</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <f>(696-138)*(1038-981)</f>
+        <v>31806</v>
+      </c>
+      <c r="G3">
+        <f>0.5*0.5</f>
+        <v>0.25</v>
+      </c>
+      <c r="H3" s="6">
+        <f>G3/F3</f>
+        <v>7.8601521725460613E-6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4">
+        <v>986</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4">
+        <f>(1212-759)*(1038-981)</f>
+        <v>25821</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G9" si="0">0.5*0.5</f>
+        <v>0.25</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4:H9" si="1">G4/F4</f>
+        <v>9.6820417489640218E-6</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="2">
+        <v>1644</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5">
+        <f>(1821-1467)*(1038-981)</f>
+        <v>20178</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2389731390623451E-5</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="K5">
+        <f>572.06-78.04</f>
+        <v>494.01999999999992</v>
+      </c>
+      <c r="L5">
+        <f>781.95-703.28</f>
+        <v>78.670000000000073</v>
+      </c>
+      <c r="M5">
+        <f>(703.28+781.95)/2</f>
+        <v>742.61500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="2">
+        <v>2232</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6">
+        <f>(2454-2010)*(1038-981)</f>
+        <v>25308</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="1"/>
+        <v>9.8782993519835626E-6</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2">
+        <v>2874</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7">
+        <f>(3162-2586)*(1038-981)</f>
+        <v>32832</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="1"/>
+        <v>7.6145224171539957E-6</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="K7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B8" s="5"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="2"/>
+      <c r="K8">
+        <f>K5*L5</f>
+        <v>38864.553400000033</v>
+      </c>
+      <c r="L8">
+        <f>G17/(G18+G19*(M5)+G20*(M5*M5))</f>
+        <v>7.7747708563198579E-5</v>
+      </c>
+      <c r="M8">
+        <f>K8*L8</f>
+        <v>3.0216299711820711</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B9" s="5"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="J14">
+        <f>978.96-714.7</f>
+        <v>264.26</v>
+      </c>
+      <c r="K14">
+        <f>652.99-606.91</f>
+        <v>46.080000000000041</v>
+      </c>
+      <c r="L14">
+        <f>J14*K14</f>
+        <v>12177.100800000011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B17" s="2">
+        <v>1644</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1.2389731390623451E-5</v>
+      </c>
+      <c r="D17">
+        <v>417</v>
+      </c>
+      <c r="E17" s="6">
+        <v>7.8601521725460613E-6</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17">
+        <v>-2.2788150560381401E-4</v>
+      </c>
+      <c r="H17">
+        <f>G17/(G18+G19*(M5)+G20*(M5*M5))</f>
+        <v>7.7747708563198579E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <v>2232</v>
+      </c>
+      <c r="C18" s="14">
+        <v>9.8782993519835626E-6</v>
+      </c>
+      <c r="D18">
+        <v>986</v>
+      </c>
+      <c r="E18" s="6">
+        <v>9.6820417489640218E-6</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18">
+        <v>-249.575444271701</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B19">
+        <v>2874</v>
+      </c>
+      <c r="C19" s="14">
+        <v>7.6145224171539957E-6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1644</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1.2389731390623451E-5</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19">
+        <v>0.60361848274124597</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D20">
+        <v>2232</v>
+      </c>
+      <c r="E20" s="14">
+        <v>9.8782993519835626E-6</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20">
+        <v>-3.6558500089469299E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D21">
+        <v>2874</v>
+      </c>
+      <c r="E21" s="14">
+        <v>7.6145224171539957E-6</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="C23" s="2"/>
+      <c r="D23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D27" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to depth estimation equation
</commit_message>
<xml_diff>
--- a/modules/area_estimation/3280x2464/ScalingFactor.xlsx
+++ b/modules/area_estimation/3280x2464/ScalingFactor.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\GitHub\ai-pothole-models\modules\area_estimation\3280x2464\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F7CC07-52CA-4755-8A31-D9C557D3CC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD9692D-F293-45C2-BAEB-2D07C2FE0A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="y-scaling factor" sheetId="1" r:id="rId1"/>
     <sheet name="x-scaling factor" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>Rectangle</t>
   </si>
@@ -184,10 +185,6 @@
     <t>CENTER COLUMN</t>
   </si>
   <si>
-    <t>x-axis distance from camera
-(pixels)</t>
-  </si>
-  <si>
     <t>(138, 981)</t>
   </si>
   <si>
@@ -216,15 +213,44 @@
   </si>
   <si>
     <t>(3162, 1038)</t>
+  </si>
+  <si>
+    <t>y-axis distance from
+camera (pixels)</t>
+  </si>
+  <si>
+    <t>Actual square
+area (m^2)</t>
+  </si>
+  <si>
+    <t>(985.5, 1010)</t>
+  </si>
+  <si>
+    <t>(417.0, 1010)</t>
+  </si>
+  <si>
+    <t>(1644.0, 1010)</t>
+  </si>
+  <si>
+    <t>(2232.0, 1010)</t>
+  </si>
+  <si>
+    <t>(2874.0, 1010)</t>
+  </si>
+  <si>
+    <t>x-axis distance from
+camera (pixels)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="170" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="172" formatCode="0.000000000000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -277,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,6 +328,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -311,7 +338,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1071,7 +1102,7 @@
             <c:numRef>
               <c:f>'x-scaling factor'!$E$17:$E$21</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000000000</c:formatCode>
+                <c:formatCode>0.00000000000000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>7.8601521725460613E-6</c:v>
@@ -1082,10 +1113,10 @@
                 <c:pt idx="2">
                   <c:v>1.2389731390623451E-5</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.0000000000000000">
+                <c:pt idx="3">
                   <c:v>9.8782993519835626E-6</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.0000000000000000">
+                <c:pt idx="4">
                   <c:v>7.6145224171539957E-6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1194,8 +1225,8 @@
                     <c:strCache>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>x-axis distance from camera
-(pixels)</c:v>
+                        <c:v>x-axis distance from
+camera (pixels)</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>417</c:v>
@@ -1219,7 +1250,7 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>0.000000000000000</c:formatCode>
+                      <c:formatCode>0.00000000000000</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0" formatCode="General">
                         <c:v>0</c:v>
@@ -1276,31 +1307,19 @@
                   </c:spPr>
                 </c:marker>
                 <c:xVal>
-                  <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:numRef>
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'x-scaling factor'!$B$16:$B$19</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                    <c:strCache>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
                       <c:ptCount val="4"/>
-                      <c:pt idx="0">
-                        <c:v>x-axis distance from camera
-(pixels)</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1644</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>2232</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>2874</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
+                    </c:numCache>
+                  </c:numRef>
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
@@ -1314,18 +1333,6 @@
                     <c:numCache>
                       <c:formatCode>0.000000000000000</c:formatCode>
                       <c:ptCount val="4"/>
-                      <c:pt idx="0" formatCode="General">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1.2389731390623451E-5</c:v>
-                      </c:pt>
-                      <c:pt idx="2" formatCode="0.0000000000000000">
-                        <c:v>9.8782993519835626E-6</c:v>
-                      </c:pt>
-                      <c:pt idx="3" formatCode="0.0000000000000000">
-                        <c:v>7.6145224171539957E-6</c:v>
-                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
@@ -1518,7 +1525,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000000000000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000000000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3064,19 +3071,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" customWidth="1"/>
-    <col min="6" max="6" width="32.73046875" customWidth="1"/>
-    <col min="7" max="7" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.59765625" bestFit="1" customWidth="1"/>
@@ -3089,8 +3096,8 @@
         <v>45</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
@@ -3100,17 +3107,17 @@
         <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>32</v>
@@ -3401,7 +3408,7 @@
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C16" s="4" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>23</v>
@@ -3412,7 +3419,7 @@
       <c r="C17">
         <v>1972</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>1.1098247009688326E-7</v>
       </c>
       <c r="F17" s="7" t="s">
@@ -3430,7 +3437,7 @@
       <c r="C18">
         <v>1158</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="12">
         <v>3.3379619739371929E-6</v>
       </c>
       <c r="F18" s="7" t="s">
@@ -3444,7 +3451,7 @@
       <c r="C19" s="2">
         <v>1006</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="12">
         <v>1.3354700854700855E-5</v>
       </c>
       <c r="F19" s="7" t="s">
@@ -3458,7 +3465,7 @@
       <c r="C20" s="2">
         <v>941</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="12">
         <v>3.908692933083177E-5</v>
       </c>
       <c r="F20" s="7" t="s">
@@ -3472,7 +3479,7 @@
       <c r="C21" s="2">
         <v>900</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="12">
         <v>1.0121457489878542E-4</v>
       </c>
       <c r="F21" s="6"/>
@@ -3481,7 +3488,7 @@
       <c r="C22" s="2">
         <v>873</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="12">
         <v>1.8037518037518038E-4</v>
       </c>
       <c r="F22" s="6"/>
@@ -3490,7 +3497,7 @@
       <c r="C23" s="2">
         <v>854</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>3.2051282051282051E-4</v>
       </c>
       <c r="F23" s="6"/>
@@ -3522,20 +3529,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1E50E9-E4C9-46DC-A3D5-132ED23BE96B}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.73046875" customWidth="1"/>
-    <col min="7" max="7" width="22.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" customWidth="1"/>
+    <col min="6" max="6" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.53125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.86328125" bestFit="1" customWidth="1"/>
@@ -3547,10 +3553,10 @@
         <v>44</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3558,17 +3564,17 @@
         <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>32</v>
@@ -3586,14 +3592,17 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="C3">
         <v>417</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3">
         <f>(696-138)*(1038-981)</f>
@@ -3603,7 +3612,7 @@
         <f>0.5*0.5</f>
         <v>0.25</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="18">
         <f>G3/F3</f>
         <v>7.8601521725460613E-6</v>
       </c>
@@ -3618,15 +3627,17 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="C4">
         <v>986</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="F4">
         <f>(1212-759)*(1038-981)</f>
@@ -3636,7 +3647,7 @@
         <f t="shared" ref="G4:G7" si="0">0.5*0.5</f>
         <v>0.25</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="18">
         <f t="shared" ref="H4:H7" si="1">G4/F4</f>
         <v>9.6820417489640218E-6</v>
       </c>
@@ -3654,15 +3665,17 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C5" s="2">
         <v>1644</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F5">
         <f>(1821-1467)*(1038-981)</f>
@@ -3672,7 +3685,7 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="18">
         <f t="shared" si="1"/>
         <v>1.2389731390623451E-5</v>
       </c>
@@ -3694,15 +3707,17 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="C6" s="2">
         <v>2232</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F6">
         <f>(2454-2010)*(1038-981)</f>
@@ -3712,7 +3727,7 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="18">
         <f t="shared" si="1"/>
         <v>9.8782993519835626E-6</v>
       </c>
@@ -3722,15 +3737,17 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="C7" s="2">
         <v>2874</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="F7">
         <f>(3162-2586)*(1038-981)</f>
@@ -3740,7 +3757,7 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="18">
         <f t="shared" si="1"/>
         <v>7.6145224171539957E-6</v>
       </c>
@@ -3803,31 +3820,23 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B17" s="2">
-        <v>1644</v>
-      </c>
-      <c r="C17" s="6">
-        <v>1.2389731390623451E-5</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="6"/>
       <c r="D17">
         <v>417</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="17">
         <v>7.8601521725460613E-6</v>
       </c>
       <c r="F17" s="7" t="s">
@@ -3842,16 +3851,11 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B18">
-        <v>2232</v>
-      </c>
-      <c r="C18" s="11">
-        <v>9.8782993519835626E-6</v>
-      </c>
+      <c r="C18" s="11"/>
       <c r="D18">
         <v>986</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="17">
         <v>9.6820417489640218E-6</v>
       </c>
       <c r="F18" s="7" t="s">
@@ -3862,16 +3866,11 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B19">
-        <v>2874</v>
-      </c>
-      <c r="C19" s="11">
-        <v>7.6145224171539957E-6</v>
-      </c>
+      <c r="C19" s="11"/>
       <c r="D19" s="2">
         <v>1644</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="17">
         <v>1.2389731390623451E-5</v>
       </c>
       <c r="F19" s="7" t="s">
@@ -3885,7 +3884,7 @@
       <c r="D20">
         <v>2232</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="17">
         <v>9.8782993519835626E-6</v>
       </c>
       <c r="F20" s="7" t="s">
@@ -3899,7 +3898,7 @@
       <c r="D21">
         <v>2874</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="17">
         <v>7.6145224171539957E-6</v>
       </c>
       <c r="F21" s="6"/>
@@ -3933,4 +3932,265 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87DADB33-5144-443F-9905-58AFB891AE3F}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" customWidth="1"/>
+    <col min="4" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1972</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f>(2816-508)*(2460-1484)</f>
+        <v>2252608</v>
+      </c>
+      <c r="G3">
+        <f>0.5*0.5</f>
+        <v>0.25</v>
+      </c>
+      <c r="H3" s="6">
+        <f>G3/F3</f>
+        <v>1.1098247009688326E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>1158</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <f>(1944-1340)*(1220-1096)</f>
+        <v>74896</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G9" si="0">0.5*0.5</f>
+        <v>0.25</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4:H9" si="1">G4/F4</f>
+        <v>3.3379619739371929E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1006</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <f>(1828-1468)*(1032-980)</f>
+        <v>18720</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3354700854700855E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
+        <v>941</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <f>(1766-1520)*(954-928)</f>
+        <v>6396</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="1"/>
+        <v>3.908692933083177E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>900</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <f>(1738-1548)*(907-894)</f>
+        <v>2470</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="1"/>
+        <v>1.0121457489878542E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2">
+        <v>873</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <f>(1718-1564)*(878-869)</f>
+        <v>1386</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="1"/>
+        <v>1.8037518037518038E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2">
+        <v>854</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <f>(1706-1576)*(857-851)</f>
+        <v>780</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="1"/>
+        <v>3.2051282051282051E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>